<commit_message>
Fix enums and imports
</commit_message>
<xml_diff>
--- a/src/tools/validate_stamina/data/stamina_calculator.xlsx
+++ b/src/tools/validate_stamina/data/stamina_calculator.xlsx
@@ -64,31 +64,37 @@
     <t>Turf</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Dirt</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Distance Apt.</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
-    <t>Dirt</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Distance Apt.</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
     <t>Mile</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>Long</t>
   </si>
   <si>
-    <t>B</t>
+    <t>G</t>
   </si>
   <si>
     <t>PLEASE MAKE A COPY! I WILL NOT SHARE ACCESS! THANK YOU &lt;3</t>
@@ -106,13 +112,10 @@
     <t>Late</t>
   </si>
   <si>
-    <t>S</t>
+    <t>E</t>
   </si>
   <si>
     <t>End</t>
-  </si>
-  <si>
-    <t>G</t>
   </si>
   <si>
     <t>Mood</t>
@@ -331,10 +334,7 @@
     <t>HP Correction</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
+    <t>C</t>
   </si>
   <si>
     <t>F</t>
@@ -3378,7 +3378,7 @@
     <xdr:ext cx="981075" cy="590550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image1.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3434,7 +3434,7 @@
     <xdr:ext cx="2581275" cy="2495550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3787,25 +3787,25 @@
     <row r="8" ht="32.25" customHeight="1">
       <c r="B8" s="9"/>
       <c r="C8" s="16">
-        <v>600.0</v>
+        <v>1088.0</v>
       </c>
       <c r="D8" s="17">
-        <v>600.0</v>
+        <v>625.0</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
       <c r="G8" s="17">
-        <v>600.0</v>
+        <v>621.0</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="15"/>
       <c r="J8" s="17">
-        <v>600.0</v>
+        <v>488.0</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
       <c r="M8" s="17">
-        <v>600.0</v>
+        <v>435.0</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="15"/>
@@ -3858,28 +3858,28 @@
         <v>16</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>17</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>12</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="L12" s="18"/>
       <c r="M12" s="19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="P12" s="11"/>
     </row>
@@ -3899,40 +3899,40 @@
       <c r="N13" s="21"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="B14" s="9"/>
       <c r="C14" s="18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I14" s="18"/>
       <c r="J14" s="19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L14" s="18"/>
       <c r="M14" s="19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="P14" s="11"/>
     </row>
@@ -3943,17 +3943,17 @@
     <row r="16">
       <c r="B16" s="9"/>
       <c r="C16" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E16" s="25"/>
       <c r="G16" s="26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K16" s="25"/>
       <c r="P16" s="11"/>
@@ -3966,7 +3966,7 @@
     <row r="18">
       <c r="B18" s="9"/>
       <c r="C18" s="27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J18" s="28">
         <v>1.0</v>
@@ -3978,7 +3978,7 @@
     <row r="19">
       <c r="B19" s="9"/>
       <c r="C19" s="30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
@@ -4031,7 +4031,7 @@
     <row r="23">
       <c r="B23" s="40"/>
       <c r="C23" s="41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="2"/>
@@ -4040,16 +4040,16 @@
     <row r="24">
       <c r="B24" s="40"/>
       <c r="C24" s="43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="31"/>
       <c r="G24" s="2"/>
       <c r="H24" s="44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="2"/>
@@ -4064,13 +4064,13 @@
       <c r="B25" s="40"/>
       <c r="C25" s="46"/>
       <c r="D25" s="47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="31"/>
       <c r="G25" s="2"/>
       <c r="H25" s="48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="49"/>
@@ -4101,7 +4101,7 @@
     <row r="27">
       <c r="B27" s="40"/>
       <c r="C27" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D27" s="31"/>
       <c r="E27" s="2"/>
@@ -4122,7 +4122,7 @@
       <c r="C28" s="50">
         <v>0.035</v>
       </c>
-      <c r="D28" s="52">
+      <c r="D28" s="51">
         <v>0.0</v>
       </c>
       <c r="E28" s="25"/>
@@ -4134,7 +4134,7 @@
       <c r="I28" s="53"/>
       <c r="J28" s="25"/>
       <c r="K28" s="55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L28" s="56"/>
       <c r="M28" s="57"/>
@@ -4145,7 +4145,7 @@
     <row r="29">
       <c r="B29" s="40"/>
       <c r="C29" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D29" s="31"/>
       <c r="E29" s="2"/>
@@ -4155,7 +4155,7 @@
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
       <c r="K29" s="59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L29" s="56"/>
       <c r="M29" s="57"/>
@@ -4180,7 +4180,7 @@
       <c r="I30" s="53"/>
       <c r="J30" s="25"/>
       <c r="K30" s="60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L30" s="57"/>
       <c r="M30" s="57"/>
@@ -4191,7 +4191,7 @@
     <row r="31">
       <c r="B31" s="40"/>
       <c r="C31" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D31" s="31"/>
       <c r="E31" s="2"/>
@@ -4210,7 +4210,7 @@
     <row r="32">
       <c r="B32" s="40"/>
       <c r="C32" s="43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D32" s="61">
         <v>0.0</v>
@@ -4233,7 +4233,7 @@
     <row r="33">
       <c r="B33" s="40"/>
       <c r="C33" s="62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="31"/>
@@ -4262,7 +4262,7 @@
     <row r="35">
       <c r="B35" s="40"/>
       <c r="C35" s="43" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D35" s="31"/>
       <c r="E35" s="31"/>
@@ -4283,7 +4283,7 @@
     <row r="36">
       <c r="B36" s="40"/>
       <c r="C36" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
@@ -4302,7 +4302,7 @@
     <row r="37">
       <c r="B37" s="40"/>
       <c r="C37" s="30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
@@ -4343,24 +4343,24 @@
     <row r="40">
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P40" s="11"/>
     </row>
     <row r="41">
       <c r="B41" s="9"/>
       <c r="C41" s="26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="25"/>
       <c r="G41" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J41" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K41" s="25"/>
       <c r="P41" s="11"/>
@@ -4368,14 +4368,14 @@
     <row r="42">
       <c r="B42" s="9"/>
       <c r="C42" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D42" s="24">
         <v>1600.0</v>
       </c>
       <c r="E42" s="25"/>
       <c r="G42" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J42" s="68" t="str">
         <f>VLOOKUP(D42,'定義'!$O$3:$P$18,2)</f>
@@ -4412,7 +4412,7 @@
     <row r="45">
       <c r="D45" s="69"/>
       <c r="H45" s="70" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" ht="7.5" customHeight="1"/>
@@ -4436,7 +4436,7 @@
     <row r="50">
       <c r="B50" s="75"/>
       <c r="C50" s="76" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P50" s="77"/>
     </row>
@@ -4461,7 +4461,7 @@
       <c r="K51" s="80"/>
       <c r="L51" s="81"/>
       <c r="M51" s="79" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N51" s="80"/>
       <c r="O51" s="81"/>
@@ -4471,29 +4471,29 @@
       <c r="B52" s="75"/>
       <c r="C52" s="82">
         <f t="array" ref="C52">(C8*VLOOKUP($D$16,'定義'!$B$23:$C$27,2, FALSE)+index('定義'!$K$13:$M$20,match($J$41,'定義'!$J$13:$J$16, 0)+if($D$41="Dirt",4,0),1))*VLOOKUP(switch($J$42,"Sprint",$E$12,"Mile",$H$12,"Medium",$K$12,"Long",$N$12),'定義'!$E$3:$G$10,2, FALSE)^2</f>
-        <v>576</v>
+        <v>1044.48</v>
       </c>
       <c r="D52" s="83">
         <f>(D8*VLOOKUP($D$16,'定義'!$B$23:$C$27,2, FALSE))</f>
-        <v>576</v>
+        <v>600</v>
       </c>
       <c r="E52" s="80"/>
       <c r="F52" s="81"/>
       <c r="G52" s="83">
         <f t="array" ref="G52">(G8*VLOOKUP($D$16,'定義'!$B$23:$C$27,2, FALSE)+index('定義'!$K$13:$M$20,match($J$41,'定義'!$J$13:$J$16, 0)+if($D$41="Dirt",4,0),2))*VLOOKUP(switch($J$42,"Sprint",$E$12,"Mile",$H$12,"Medium",$K$12,"Long",$N$12),'定義'!$E$3:$G$10,3, FALSE)^2*VLOOKUP(switch($D$41,"Turf",$E$10,"Dirt",$H$10),'定義'!$B$3:$C$10,2, FALSE)^2</f>
-        <v>576</v>
+        <v>657.2664</v>
       </c>
       <c r="H52" s="80"/>
       <c r="I52" s="81"/>
       <c r="J52" s="83">
         <f>(J8*VLOOKUP($D$16,'定義'!$B$23:$C$27,2, FALSE))</f>
-        <v>576</v>
+        <v>468.48</v>
       </c>
       <c r="K52" s="80"/>
       <c r="L52" s="81"/>
       <c r="M52" s="83">
         <f>(M8*VLOOKUP($D$16,'定義'!$B$23:$C$27,2, FALSE))*VLOOKUP(switch($J$16,"Front",$E$14,"Pace",$H$14,"Late",$K$14,"End",$N$14),'定義'!$I$3:$J$10,2, FALSE)</f>
-        <v>633.6</v>
+        <v>417.6</v>
       </c>
       <c r="N52" s="80"/>
       <c r="O52" s="81"/>
@@ -4506,16 +4506,16 @@
     <row r="54" ht="20.25" customHeight="1">
       <c r="B54" s="75"/>
       <c r="C54" s="84" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D54" s="85" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E54" s="86"/>
       <c r="F54" s="87"/>
       <c r="G54" s="88" t="str">
         <f>IF(D52+1&lt;D55,"Not enough stamina/guts！",IF(and(D52/D55&lt;1.1,D55&gt;=0),"Borderline！","You have enough！"))</f>
-        <v>You have enough！</v>
+        <v>Borderline！</v>
       </c>
       <c r="H54" s="89"/>
       <c r="I54" s="89"/>
@@ -4531,7 +4531,7 @@
       <c r="B55" s="75"/>
       <c r="D55" s="91">
         <f>'定義'!G57</f>
-        <v>453.9335406</v>
+        <v>570.2203876</v>
       </c>
       <c r="E55" s="86"/>
       <c r="F55" s="87"/>
@@ -4557,20 +4557,20 @@
     <row r="57" ht="45.75" customHeight="1">
       <c r="B57" s="75"/>
       <c r="C57" s="97" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D57" s="98">
         <f>max(100-9000/M52,20)/100</f>
-        <v>0.8579545455</v>
+        <v>0.7844827586</v>
       </c>
       <c r="E57" s="80"/>
       <c r="F57" s="81"/>
       <c r="G57" s="97" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J57" s="98">
         <f>MIN((6.5/LOG10(0.1*M52+1))^2/100, 1)</f>
-        <v>0.1291617615</v>
+        <v>0.1588176319</v>
       </c>
       <c r="K57" s="80"/>
       <c r="L57" s="81"/>
@@ -4619,45 +4619,45 @@
     <row r="61">
       <c r="B61" s="75"/>
       <c r="C61" s="102" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S61" s="77"/>
     </row>
     <row r="62">
       <c r="B62" s="75"/>
       <c r="C62" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D62" s="103">
         <f>'定義'!B34</f>
-        <v>2060.8</v>
+        <v>2027.2</v>
       </c>
       <c r="E62" s="81"/>
       <c r="G62" s="26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J62" s="103">
         <f>'定義'!B30</f>
-        <v>91.15749338</v>
+        <v>90.83705562</v>
       </c>
       <c r="K62" s="81"/>
       <c r="L62" s="104" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S62" s="77"/>
     </row>
     <row r="63">
       <c r="B63" s="75"/>
       <c r="C63" s="26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D63" s="103">
         <f>'定義'!B35</f>
-        <v>2060.8</v>
+        <v>2027.2</v>
       </c>
       <c r="E63" s="81"/>
       <c r="G63" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J63" s="103">
         <f>'定義'!B31</f>
@@ -4665,22 +4665,22 @@
       </c>
       <c r="K63" s="81"/>
       <c r="L63" s="104" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S63" s="77"/>
     </row>
     <row r="64">
       <c r="B64" s="75"/>
       <c r="C64" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D64" s="105">
         <f>'定義'!B37</f>
-        <v>1.340206909</v>
+        <v>1.377232275</v>
       </c>
       <c r="E64" s="81"/>
       <c r="G64" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J64" s="106">
         <f>'定義'!B33</f>
@@ -4688,7 +4688,7 @@
       </c>
       <c r="K64" s="81"/>
       <c r="L64" s="104" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S64" s="77"/>
     </row>
@@ -4700,38 +4700,38 @@
       <c r="B66" s="75"/>
       <c r="C66" s="26"/>
       <c r="D66" s="107" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E66" s="108"/>
       <c r="F66" s="109"/>
       <c r="G66" s="107" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H66" s="108"/>
       <c r="I66" s="109"/>
       <c r="J66" s="107" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K66" s="108"/>
       <c r="L66" s="109"/>
       <c r="M66" s="107" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N66" s="108"/>
       <c r="O66" s="109"/>
       <c r="P66" s="107" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q66" s="109"/>
       <c r="R66" s="110" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S66" s="77"/>
     </row>
     <row r="67">
       <c r="B67" s="75"/>
       <c r="C67" s="111" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D67" s="112">
         <f>'定義'!B41</f>
@@ -4747,31 +4747,31 @@
       <c r="I67" s="109"/>
       <c r="J67" s="112">
         <f>'定義'!D41</f>
-        <v>24.31394394</v>
+        <v>24.33879984</v>
       </c>
       <c r="K67" s="108"/>
       <c r="L67" s="109"/>
       <c r="M67" s="112">
         <f>'定義'!E41</f>
-        <v>0.5897850235</v>
+        <v>0.589182708</v>
       </c>
       <c r="N67" s="108"/>
       <c r="O67" s="109"/>
       <c r="P67" s="113">
         <f>'定義'!F41</f>
-        <v>5.998113689</v>
+        <v>5.99198814</v>
       </c>
       <c r="Q67" s="109"/>
       <c r="R67" s="114">
         <f>'定義'!G41</f>
-        <v>11.79570047</v>
+        <v>11.78365416</v>
       </c>
       <c r="S67" s="77"/>
     </row>
     <row r="68">
       <c r="B68" s="75"/>
       <c r="C68" s="111" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D68" s="112">
         <f>'定義'!B42</f>
@@ -4781,41 +4781,41 @@
       <c r="F68" s="109"/>
       <c r="G68" s="112">
         <f>'定義'!C42</f>
-        <v>19.1112441</v>
+        <v>19.91000422</v>
       </c>
       <c r="H68" s="108"/>
       <c r="I68" s="109"/>
       <c r="J68" s="112">
         <f>'定義'!D42</f>
-        <v>0.313943944</v>
+        <v>0.3387998417</v>
       </c>
       <c r="K68" s="108"/>
       <c r="L68" s="109"/>
       <c r="M68" s="112">
         <f>'定義'!E42</f>
-        <v>5.641911977</v>
+        <v>7.585612235</v>
       </c>
       <c r="N68" s="108"/>
       <c r="O68" s="109"/>
       <c r="P68" s="113">
         <f>'定義'!F42</f>
-        <v>102.8273553</v>
+        <v>141.2820439</v>
       </c>
       <c r="Q68" s="109"/>
       <c r="R68" s="114">
         <f>'定義'!G42</f>
-        <v>75.85573439</v>
+        <v>110.7300036</v>
       </c>
       <c r="S68" s="77"/>
     </row>
     <row r="69">
       <c r="B69" s="75"/>
       <c r="C69" s="111" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D69" s="112">
         <f>'定義'!B43</f>
-        <v>19.1112441</v>
+        <v>19.91000422</v>
       </c>
       <c r="E69" s="108"/>
       <c r="F69" s="108"/>
@@ -4830,69 +4830,69 @@
       <c r="L69" s="109"/>
       <c r="M69" s="112">
         <f>'定義'!E43</f>
-        <v>8.259074964</v>
+        <v>5.996615233</v>
       </c>
       <c r="N69" s="108"/>
       <c r="O69" s="109"/>
       <c r="P69" s="113">
         <f>'定義'!F43</f>
-        <v>157.8411977</v>
+        <v>119.3926346</v>
       </c>
       <c r="Q69" s="109"/>
       <c r="R69" s="114">
         <f>'定義'!G43</f>
-        <v>131.6069258</v>
+        <v>110.3378846</v>
       </c>
       <c r="S69" s="77"/>
     </row>
     <row r="70">
       <c r="B70" s="75"/>
       <c r="C70" s="111" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D70" s="112">
         <f>'定義'!B44</f>
-        <v>19.1112441</v>
+        <v>19.91000422</v>
       </c>
       <c r="E70" s="108"/>
       <c r="F70" s="109"/>
       <c r="G70" s="112">
         <f>'定義'!C44</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="H70" s="108"/>
       <c r="I70" s="109"/>
       <c r="J70" s="112">
         <f>'定義'!D44</f>
-        <v>0.3219937888</v>
+        <v>0.3439592301</v>
       </c>
       <c r="K70" s="108"/>
       <c r="L70" s="109"/>
       <c r="M70" s="112">
         <f>'定義'!E44</f>
-        <v>3.710628295</v>
+        <v>0.6864758861</v>
       </c>
       <c r="N70" s="108"/>
       <c r="O70" s="109"/>
       <c r="P70" s="113">
         <f>'定義'!F44</f>
-        <v>73.13145108</v>
+        <v>13.74878304</v>
       </c>
       <c r="Q70" s="109"/>
       <c r="R70" s="114">
         <f>'定義'!G44</f>
-        <v>65.96898518</v>
+        <v>12.89206675</v>
       </c>
       <c r="S70" s="77"/>
     </row>
     <row r="71">
       <c r="B71" s="75"/>
       <c r="C71" s="111" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D71" s="112">
         <f>'定義'!B45</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="E71" s="108"/>
       <c r="F71" s="108"/>
@@ -4907,41 +4907,41 @@
       <c r="L71" s="109"/>
       <c r="M71" s="112">
         <f>'定義'!E45</f>
-        <v>35.795676</v>
+        <v>39.02741883</v>
       </c>
       <c r="N71" s="108"/>
       <c r="O71" s="109"/>
       <c r="P71" s="113">
         <f>'定義'!F45</f>
-        <v>726.8685489</v>
+        <v>786.251217</v>
       </c>
       <c r="Q71" s="109"/>
       <c r="R71" s="114">
         <f>'定義'!G45</f>
-        <v>758.5327419</v>
+        <v>799.5430048</v>
       </c>
       <c r="S71" s="77"/>
     </row>
     <row r="72">
       <c r="B72" s="75"/>
       <c r="C72" s="111" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D72" s="112">
         <f>'定義'!B46</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="E72" s="108"/>
       <c r="F72" s="109"/>
       <c r="G72" s="112">
         <f>'定義'!C46</f>
-        <v>21.32695673</v>
+        <v>21.29412772</v>
       </c>
       <c r="H72" s="108"/>
       <c r="I72" s="109"/>
       <c r="J72" s="112">
         <f>'定義'!D46</f>
-        <v>0.3219937888</v>
+        <v>0.3425833932</v>
       </c>
       <c r="K72" s="108"/>
       <c r="L72" s="109"/>
@@ -4965,11 +4965,11 @@
     <row r="73">
       <c r="B73" s="75"/>
       <c r="C73" s="111" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D73" s="112">
         <f>'定義'!B47</f>
-        <v>21.32695673</v>
+        <v>21.29412772</v>
       </c>
       <c r="E73" s="108"/>
       <c r="F73" s="108"/>
@@ -5002,51 +5002,51 @@
     <row r="74">
       <c r="B74" s="75"/>
       <c r="C74" s="111" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D74" s="112">
         <f>'定義'!B48</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="E74" s="108"/>
       <c r="F74" s="109"/>
       <c r="G74" s="112">
         <f>'定義'!C48</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="H74" s="108"/>
       <c r="I74" s="109"/>
       <c r="J74" s="112">
         <f>'定義'!D48</f>
-        <v>0.3219937888</v>
+        <v>0.3425833932</v>
       </c>
       <c r="K74" s="108"/>
       <c r="L74" s="109"/>
       <c r="M74" s="112">
         <f>'定義'!E48</f>
-        <v>10.55898482</v>
+        <v>11.42930246</v>
       </c>
       <c r="N74" s="108"/>
       <c r="O74" s="109"/>
       <c r="P74" s="113">
         <f>'定義'!F48</f>
-        <v>232.3610952</v>
+        <v>252.6317992</v>
       </c>
       <c r="Q74" s="109"/>
       <c r="R74" s="114">
         <f>'定義'!G48</f>
-        <v>365.7437451</v>
+        <v>413.3570199</v>
       </c>
       <c r="S74" s="77"/>
     </row>
     <row r="75">
       <c r="B75" s="75"/>
       <c r="C75" s="111" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D75" s="112">
         <f>'定義'!B49</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="E75" s="108"/>
       <c r="F75" s="108"/>
@@ -5061,34 +5061,34 @@
       <c r="L75" s="109"/>
       <c r="M75" s="112">
         <f>'定義'!E49</f>
-        <v>12.69605196</v>
+        <v>11.66594826</v>
       </c>
       <c r="N75" s="108"/>
       <c r="O75" s="109"/>
       <c r="P75" s="113">
         <f>'定義'!F49</f>
-        <v>300.9722381</v>
+        <v>280.7015341</v>
       </c>
       <c r="Q75" s="109"/>
       <c r="R75" s="114">
         <f>'定義'!G49</f>
-        <v>553.6429997</v>
+        <v>547.3532822</v>
       </c>
       <c r="S75" s="77"/>
     </row>
     <row r="76">
       <c r="B76" s="75"/>
       <c r="C76" s="111" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D76" s="112">
         <f>'定義'!B50</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="E76" s="108"/>
       <c r="F76" s="109"/>
       <c r="G76" s="115" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H76" s="108"/>
       <c r="I76" s="109"/>
@@ -5118,11 +5118,11 @@
     <row r="77">
       <c r="B77" s="75"/>
       <c r="C77" s="111" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M77" s="112">
         <f>'定義'!E51</f>
-        <v>77.25211303</v>
+        <v>76.98055561</v>
       </c>
       <c r="N77" s="108"/>
       <c r="O77" s="109"/>
@@ -5133,7 +5133,7 @@
       <c r="Q77" s="109"/>
       <c r="R77" s="114">
         <f>'定義'!G51</f>
-        <v>1963.146833</v>
+        <v>2005.996916</v>
       </c>
       <c r="S77" s="77"/>
     </row>
@@ -5360,7 +5360,7 @@
   <sheetData>
     <row r="1" ht="36.75" customHeight="1">
       <c r="A1" s="121" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
@@ -5369,45 +5369,45 @@
         <v>10</v>
       </c>
       <c r="C2" s="123" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="123" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F2" s="123" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G2" s="123" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H2" s="31"/>
       <c r="I2" s="123" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J2" s="123" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O2" s="123" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P2" s="123" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R2" s="122"/>
       <c r="S2" s="123" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T2" s="123" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="U2" s="124" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="V2" s="53"/>
       <c r="W2" s="25"/>
       <c r="X2" s="124" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Y2" s="53"/>
       <c r="Z2" s="25"/>
@@ -5415,14 +5415,14 @@
     <row r="3">
       <c r="A3" s="125"/>
       <c r="B3" s="126" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C3" s="126">
         <v>1.05</v>
       </c>
       <c r="D3" s="31"/>
       <c r="E3" s="126" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F3" s="126">
         <v>1.05</v>
@@ -5432,7 +5432,7 @@
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="126" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="J3" s="126">
         <v>1.1</v>
@@ -5445,7 +5445,7 @@
       </c>
       <c r="R3" s="122"/>
       <c r="S3" s="128" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="T3" s="126">
         <v>0.95</v>
@@ -5472,14 +5472,14 @@
     <row r="4">
       <c r="A4" s="125"/>
       <c r="B4" s="126" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" s="126">
         <v>1.0</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="126" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F4" s="126">
         <v>1.0</v>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="H4" s="31"/>
       <c r="I4" s="126" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J4" s="126">
         <v>1.0</v>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="R4" s="122"/>
       <c r="S4" s="128" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="T4" s="126">
         <v>0.89</v>
@@ -5529,14 +5529,14 @@
     <row r="5">
       <c r="A5" s="125"/>
       <c r="B5" s="126" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5" s="126">
         <v>0.9</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="126" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F5" s="126">
         <v>0.9</v>
@@ -5546,7 +5546,7 @@
       </c>
       <c r="H5" s="31"/>
       <c r="I5" s="126" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J5" s="126">
         <v>0.85</v>
@@ -5559,7 +5559,7 @@
       </c>
       <c r="R5" s="122"/>
       <c r="S5" s="128" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="T5" s="126">
         <v>1.0</v>
@@ -5586,14 +5586,14 @@
     <row r="6">
       <c r="A6" s="125"/>
       <c r="B6" s="126" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="C6" s="126">
         <v>0.8</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="126" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="F6" s="126">
         <v>0.8</v>
@@ -5603,7 +5603,7 @@
       </c>
       <c r="H6" s="31"/>
       <c r="I6" s="126" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="J6" s="126">
         <v>0.75</v>
@@ -5612,11 +5612,11 @@
         <v>1500.0</v>
       </c>
       <c r="P6" s="127" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R6" s="122"/>
       <c r="S6" s="128" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T6" s="126">
         <v>0.995</v>
@@ -5643,14 +5643,14 @@
     <row r="7">
       <c r="A7" s="125"/>
       <c r="B7" s="126" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C7" s="126">
         <v>0.7</v>
       </c>
       <c r="D7" s="31"/>
       <c r="E7" s="126" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F7" s="126">
         <v>0.6</v>
@@ -5660,7 +5660,7 @@
       </c>
       <c r="H7" s="31"/>
       <c r="I7" s="126" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="J7" s="126">
         <v>0.6</v>
@@ -5669,20 +5669,20 @@
         <v>1600.0</v>
       </c>
       <c r="P7" s="127" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="125"/>
       <c r="B8" s="126" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C8" s="126">
         <v>0.5</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="126" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="F8" s="126">
         <v>0.4</v>
@@ -5692,7 +5692,7 @@
       </c>
       <c r="H8" s="31"/>
       <c r="I8" s="126" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="J8" s="126">
         <v>0.4</v>
@@ -5701,7 +5701,7 @@
         <v>1800.0</v>
       </c>
       <c r="P8" s="127" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -5733,7 +5733,7 @@
         <v>2000.0</v>
       </c>
       <c r="P9" s="127" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U9" s="129">
         <f t="shared" ref="U9:U12" si="1">U3/6</f>
@@ -5755,14 +5755,14 @@
     <row r="10">
       <c r="A10" s="125"/>
       <c r="B10" s="126" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C10" s="126">
         <v>0.1</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="126" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F10" s="126">
         <v>0.1</v>
@@ -5772,7 +5772,7 @@
       </c>
       <c r="H10" s="31"/>
       <c r="I10" s="126" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J10" s="126">
         <v>0.1</v>
@@ -5781,7 +5781,7 @@
         <v>2200.0</v>
       </c>
       <c r="P10" s="127" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U10" s="129">
         <f t="shared" si="1"/>
@@ -5805,7 +5805,7 @@
         <v>2300.0</v>
       </c>
       <c r="P11" s="127" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U11" s="129">
         <f t="shared" si="1"/>
@@ -5832,7 +5832,7 @@
         <v>104</v>
       </c>
       <c r="E12" s="130" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F12" s="130" t="s">
         <v>104</v>
@@ -5841,7 +5841,7 @@
         <v>103</v>
       </c>
       <c r="J12" s="123" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K12" s="123" t="s">
         <v>105</v>
@@ -5856,7 +5856,7 @@
         <v>2400.0</v>
       </c>
       <c r="P12" s="127" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U12" s="129">
         <f t="shared" si="1"/>
@@ -5883,7 +5883,7 @@
         <v>1.0</v>
       </c>
       <c r="E13" s="128" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F13" s="126">
         <v>1.0</v>
@@ -5892,7 +5892,7 @@
         <v>11</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K13" s="126">
         <v>0.0</v>
@@ -5907,7 +5907,7 @@
         <v>2500.0</v>
       </c>
       <c r="P13" s="127" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -5940,7 +5940,7 @@
         <v>2600.0</v>
       </c>
       <c r="P14" s="127" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
@@ -5969,7 +5969,7 @@
         <v>3000.0</v>
       </c>
       <c r="P15" s="127" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -5996,7 +5996,7 @@
         <v>3200.0</v>
       </c>
       <c r="P16" s="127" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
@@ -6004,7 +6004,7 @@
         <v>13</v>
       </c>
       <c r="J17" s="128" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K17" s="126">
         <v>0.0</v>
@@ -6019,7 +6019,7 @@
         <v>3400.0</v>
       </c>
       <c r="P17" s="127" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="S17" s="122"/>
       <c r="T17" s="125"/>
@@ -6048,7 +6048,7 @@
         <v>3600.0</v>
       </c>
       <c r="P18" s="127" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="S18" s="122"/>
       <c r="T18" s="125"/>
@@ -6207,7 +6207,7 @@
     <row r="27">
       <c r="A27" s="122"/>
       <c r="B27" s="128" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C27" s="128">
         <v>0.96</v>
@@ -6245,10 +6245,10 @@
       </c>
       <c r="B30" s="136">
         <f> 1.18 * B38</f>
-        <v>91.15749338</v>
+        <v>90.83705562</v>
       </c>
       <c r="C30" s="126" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="137" t="s">
         <v>118</v>
@@ -6266,7 +6266,7 @@
         <v>533.3333333</v>
       </c>
       <c r="C31" s="126" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D31" s="139"/>
       <c r="E31" s="139"/>
@@ -6288,7 +6288,7 @@
         <v>20.4</v>
       </c>
       <c r="C33" s="126" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D33" s="31"/>
       <c r="E33" s="137" t="s">
@@ -6314,7 +6314,7 @@
       </c>
       <c r="B34" s="145">
         <f> '入力_出力'!$D$42 + 0.8 * F35 * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 2, FALSE)</f>
-        <v>2060.8</v>
+        <v>2027.2</v>
       </c>
       <c r="C34" s="31"/>
       <c r="D34" s="31"/>
@@ -6323,7 +6323,7 @@
       </c>
       <c r="F34" s="139">
         <f t="array" ref="F34">'入力_出力'!$C$8  * VLOOKUP('入力_出力'!$D$16,'定義'!$B$23:$C$27,2, FALSE)+index('定義'!$K$13:$M$20,match('入力_出力'!$J$41,'定義'!$J$13:$J$16, 0)+if('入力_出力'!$D$41="Dirt",4,0),1)</f>
-        <v>576</v>
+        <v>1044.48</v>
       </c>
       <c r="G34" s="31"/>
       <c r="I34" s="141" t="s">
@@ -6344,7 +6344,7 @@
       </c>
       <c r="B35" s="145">
         <f> B34 * (1 + (K33+K34) / 10000)</f>
-        <v>2060.8</v>
+        <v>2027.2</v>
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
@@ -6353,7 +6353,7 @@
       </c>
       <c r="F35" s="139">
         <f>'入力_出力'!$D$8  * VLOOKUP('入力_出力'!$D$16,'定義'!$B$23:$C$27,2, FALSE)</f>
-        <v>576</v>
+        <v>600</v>
       </c>
       <c r="G35" s="31"/>
     </row>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="F36" s="139">
         <f t="array" ref="F36">'入力_出力'!$G$8  * VLOOKUP('入力_出力'!$D$16,'定義'!$B$23:$C$27,2, FALSE)+index('定義'!$K$13:$M$20,match('入力_出力'!$J$41,'定義'!$J$13:$J$16, 0)+if('入力_出力'!$D$41="Dirt",4,0),2)</f>
-        <v>576</v>
+        <v>596.16</v>
       </c>
       <c r="G36" s="31"/>
     </row>
@@ -6382,7 +6382,7 @@
       </c>
       <c r="B37" s="148">
         <f> 1 + (200 / sqrt(600 * F37))</f>
-        <v>1.340206909</v>
+        <v>1.377232275</v>
       </c>
       <c r="C37" s="31"/>
       <c r="D37" s="31"/>
@@ -6391,7 +6391,7 @@
       </c>
       <c r="F37" s="139">
         <f>'入力_出力'!$J$8  * VLOOKUP('入力_出力'!$D$16,'定義'!$B$23:$C$27,2, FALSE)</f>
-        <v>576</v>
+        <v>468.48</v>
       </c>
       <c r="G37" s="31"/>
     </row>
@@ -6401,10 +6401,10 @@
       </c>
       <c r="B38" s="136">
         <f> sum(E41:E50)</f>
-        <v>77.25211303</v>
+        <v>76.98055561</v>
       </c>
       <c r="C38" s="126" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D38" s="31"/>
       <c r="E38" s="126" t="s">
@@ -6412,7 +6412,7 @@
       </c>
       <c r="F38" s="139">
         <f>'入力_出力'!$M$8  * VLOOKUP('入力_出力'!$D$16,'定義'!$B$23:$C$27,2, FALSE)*VLOOKUP(switch('入力_出力'!$J$16,"Front",'入力_出力'!$E$14,"Pace",'入力_出力'!$H$14,"Late",'入力_出力'!$K$14,"End",'入力_出力'!$N$14),'定義'!$I$3:$J$10,2, FALSE)</f>
-        <v>633.6</v>
+        <v>417.6</v>
       </c>
       <c r="G38" s="31"/>
     </row>
@@ -6452,7 +6452,7 @@
       <c r="K40" s="25"/>
       <c r="L40" s="150">
         <f>(B33 * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 4, FALSE) + ((F38 / 5500) * log10(F38 * 0.1) - 0.65 / 2) * 0.01 * B33)</f>
-        <v>20.3352441</v>
+        <v>20.17520422</v>
       </c>
     </row>
     <row r="41">
@@ -6468,19 +6468,19 @@
       </c>
       <c r="D41" s="148">
         <f> 24 + 0.0006 * sqrt(500 * F36) * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 6, FALSE) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,3, FALSE) * VLOOKUP(switch('入力_出力'!$D$41,"Turf",'入力_出力'!$E$10,"Dirt",'入力_出力'!$H$10),'定義'!$B$3:$C$10,2, FALSE)</f>
-        <v>24.31394394</v>
+        <v>24.33879984</v>
       </c>
       <c r="E41" s="148">
         <f> (C41 - B41) / D41</f>
-        <v>0.5897850235</v>
+        <v>0.589182708</v>
       </c>
       <c r="F41" s="140">
         <f> (B41 + C41) / 2 * E41</f>
-        <v>5.998113689</v>
+        <v>5.99198814</v>
       </c>
       <c r="G41" s="140">
         <f> 20 * B36 * E41</f>
-        <v>11.79570047</v>
+        <v>11.78365416</v>
       </c>
       <c r="I41" s="149" t="s">
         <v>144</v>
@@ -6489,7 +6489,7 @@
       <c r="K41" s="25"/>
       <c r="L41" s="151">
         <f>('入力_出力'!D42/24/L40)/('入力_出力'!D42/24/L40+3)</f>
-        <v>0.5221697658</v>
+        <v>0.5241408285</v>
       </c>
       <c r="M41" s="152" t="s">
         <v>145</v>
@@ -6511,23 +6511,23 @@
       </c>
       <c r="C42" s="148">
         <f> B43</f>
-        <v>19.1112441</v>
+        <v>19.91000422</v>
       </c>
       <c r="D42" s="148">
         <f> 0.0006 * sqrt(500 * F36) * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 6, FALSE) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,3, FALSE) * VLOOKUP(switch('入力_出力'!$D$41,"Turf",'入力_出力'!$E$10,"Dirt",'入力_出力'!$H$10),'定義'!$B$3:$C$10,2, FALSE)</f>
-        <v>0.313943944</v>
+        <v>0.3387998417</v>
       </c>
       <c r="E42" s="148">
         <f> min((C42 - B42) / D42, (-B42 + sqrt(B42 ^ 2 + 2 * D42 * ('入力_出力'!D42 / 6 - F41))) / D42)</f>
-        <v>5.641911977</v>
+        <v>7.585612235</v>
       </c>
       <c r="F42" s="140">
         <f> (B42 + D42 * E42 / 2) * E42</f>
-        <v>102.8273553</v>
+        <v>141.2820439</v>
       </c>
       <c r="G42" s="140">
         <f> 20 * B36 * ((D42 * E42 + B42 - B33 + 12) ^ 3 - (B42 - B33 + 12) ^ 3) / (3 * D42) / 144</f>
-        <v>75.85573439</v>
+        <v>110.7300036</v>
       </c>
       <c r="I42" s="149" t="s">
         <v>147</v>
@@ -6544,23 +6544,23 @@
       </c>
       <c r="B43" s="153">
         <f> B33 * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 3, FALSE) + ((F38 / 5500) * log10(F38 * 0.1) - 0.65 / 2) * 0.01 * B33</f>
-        <v>19.1112441</v>
+        <v>19.91000422</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="148" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E43" s="148">
         <f> F43 / B43</f>
-        <v>8.259074964</v>
+        <v>5.996615233</v>
       </c>
       <c r="F43" s="140">
         <f> max('入力_出力'!D42 / 6 - (F41 + F42), 0)</f>
-        <v>157.8411977</v>
+        <v>119.3926346</v>
       </c>
       <c r="G43" s="140">
         <f> 20 * B36 * (B43 - B33 + 12) ^ 2 / 144 * E43</f>
-        <v>131.6069258</v>
+        <v>110.3378846</v>
       </c>
     </row>
     <row r="44">
@@ -6569,27 +6569,27 @@
       </c>
       <c r="B44" s="148">
         <f> B42 + D42 * E42</f>
-        <v>19.1112441</v>
+        <v>19.91000422</v>
       </c>
       <c r="C44" s="148">
         <f> B45</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="D44" s="148">
         <f> if(B44 &lt;= C44, 0.0006 * sqrt(500 * F36) * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 7, FALSE) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,3, FALSE) * VLOOKUP(switch('入力_出力'!$D$41,"Turf",'入力_出力'!$E$10,"Dirt",'入力_出力'!$H$10),'定義'!$B$3:$C$10,2, FALSE), -0.8)</f>
-        <v>0.3219937888</v>
+        <v>0.3439592301</v>
       </c>
       <c r="E44" s="148">
         <f> (C44 - B44) / D44</f>
-        <v>3.710628295</v>
+        <v>0.6864758861</v>
       </c>
       <c r="F44" s="140">
         <f> (B44 + C44) / 2 * E44</f>
-        <v>73.13145108</v>
+        <v>13.74878304</v>
       </c>
       <c r="G44" s="140">
         <f> 20 * B36 * ((C44 - B33 + 12) ^ 3 - (B44 - B33 + 12) ^ 3) / (3 * D44) / 144</f>
-        <v>65.96898518</v>
+        <v>12.89206675</v>
       </c>
     </row>
     <row r="45">
@@ -6598,23 +6598,23 @@
       </c>
       <c r="B45" s="154">
         <f> (B33 * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 4, FALSE) + ((F38 / 5500) * log10(F38 * 0.1) - 0.65 / 2) * 0.01 * B33) * (1 + L41*IF('入力_出力'!J16&lt;&gt;"Front", -0.055*L42, 0.04*0.2*LOG10(F38*0.1)))</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="148" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E45" s="148">
         <f> F45 / B45</f>
-        <v>35.795676</v>
+        <v>39.02741883</v>
       </c>
       <c r="F45" s="140">
         <f> '入力_出力'!D42/ 2 - F44</f>
-        <v>726.8685489</v>
+        <v>786.251217</v>
       </c>
       <c r="G45" s="155">
         <f> (20 * B36 * (B45 - B33 + 12) ^ 2 / 144 * E45) * (1 + IF(AND('入力_出力'!J18&lt;&gt;1, '入力_出力'!J18&lt;&gt;0), '入力_出力'!J57, '入力_出力'!J18)*(3*0.55+6*0.45*0.55+9*0.45^2*0.55+12*0.45^3)/E45*0.6) * IF('入力_出力'!J16&lt;&gt;"Front", (1-0.4*L42*L41), 1)</f>
-        <v>758.5327419</v>
+        <v>799.5430048</v>
       </c>
       <c r="H45" s="144" t="s">
         <v>151</v>
@@ -6632,15 +6632,15 @@
       </c>
       <c r="B46" s="148">
         <f> B45</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="C46" s="148">
         <f> B47</f>
-        <v>21.32695673</v>
+        <v>21.29412772</v>
       </c>
       <c r="D46" s="157">
         <f> if(B46 &lt;= C46, 0.0006 * sqrt(500 * F36) * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 8, FALSE) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,3, FALSE) * VLOOKUP(switch('入力_出力'!$D$41,"Turf",'入力_出力'!$E$10,"Dirt",'入力_出力'!$H$10),'定義'!$B$3:$C$10,2, FALSE), -0.8)</f>
-        <v>0.3219937888</v>
+        <v>0.3425833932</v>
       </c>
       <c r="E46" s="148">
         <f> if('入力_出力'!D42 / 3 &lt;= B31, 0, (C46 - B46) / D46)</f>
@@ -6668,11 +6668,11 @@
       </c>
       <c r="B47" s="153">
         <f> B33 * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 5, FALSE)  + sqrt(500 * F34) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,2, FALSE) * 0.002 + ((F38 / 5500) * log10(F38 * 0.1) - 0.65 / 2) * 0.01 * B33</f>
-        <v>21.32695673</v>
+        <v>21.29412772</v>
       </c>
       <c r="C47" s="25"/>
       <c r="D47" s="157" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E47" s="148">
         <f> F47 / B47</f>
@@ -6693,27 +6693,27 @@
       </c>
       <c r="B48" s="148">
         <f> if(F46 = 0, B45, B47)</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="C48" s="148">
         <f> B49</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="D48" s="157">
         <f>0.0006 * sqrt(500 * F36) * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 8, FALSE) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,3, FALSE) * VLOOKUP(switch('入力_出力'!$D$41,"Turf",'入力_出力'!$E$10,"Dirt",'入力_出力'!$H$10),'定義'!$B$3:$C$10,2, FALSE)</f>
-        <v>0.3219937888</v>
+        <v>0.3425833932</v>
       </c>
       <c r="E48" s="148">
         <f> (C48 - B48) / D48</f>
-        <v>10.55898482</v>
+        <v>11.42930246</v>
       </c>
       <c r="F48" s="140">
         <f> (B48 + C48) / 2 * E48</f>
-        <v>232.3610952</v>
+        <v>252.6317992</v>
       </c>
       <c r="G48" s="140">
         <f> 20 * B36 * B37 * ((B48 + D48 * E48 - B33 + 12) ^ 3 - (B48 - B33 + 12) ^ 3) / (3 * D48) / 144</f>
-        <v>365.7437451</v>
+        <v>413.3570199</v>
       </c>
     </row>
     <row r="49">
@@ -6722,23 +6722,23 @@
       </c>
       <c r="B49" s="153">
         <f> (B33 * (vlookup('入力_出力'!$J$16,$S$3:$Z$6, 5, FALSE) + 0.01) + sqrt(500 * F34) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,2, FALSE) * 0.002) * 1.05 + sqrt(500 * F34) *VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,2, FALSE) * 0.002</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="C49" s="25"/>
       <c r="D49" s="157" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E49" s="148">
         <f> G49 / (20 * B36 * B37 * (B49 - B33 + 12) ^ 2 / 144)</f>
-        <v>12.69605196</v>
+        <v>11.66594826</v>
       </c>
       <c r="F49" s="140">
         <f> B49 * E49</f>
-        <v>300.9722381</v>
+        <v>280.7015341</v>
       </c>
       <c r="G49" s="140">
         <f> min(20 * B36 * B37 * (B49 - B33 + 12) ^ 2 / 144 * ('入力_出力'!D42 / 3 - sum(F46:F48)) / B49, B35 - sum(G41:G48))</f>
-        <v>553.6429997</v>
+        <v>547.3532822</v>
       </c>
     </row>
     <row r="50">
@@ -6747,7 +6747,7 @@
       </c>
       <c r="B50" s="148">
         <f> B49</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="C50" s="148"/>
       <c r="D50" s="148">
@@ -6774,7 +6774,7 @@
       </c>
       <c r="E51" s="148">
         <f t="shared" ref="E51:G51" si="5"> sum(E41:E50)</f>
-        <v>77.25211303</v>
+        <v>76.98055561</v>
       </c>
       <c r="F51" s="140">
         <f t="shared" si="5"/>
@@ -6782,7 +6782,7 @@
       </c>
       <c r="G51" s="140">
         <f t="shared" si="5"/>
-        <v>1963.146833</v>
+        <v>2005.996916</v>
       </c>
     </row>
     <row r="54">
@@ -6791,27 +6791,27 @@
       </c>
       <c r="B54" s="148">
         <f>B45</f>
-        <v>20.30604336</v>
+        <v>20.14612394</v>
       </c>
       <c r="C54" s="148">
         <f> B55</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="D54" s="157">
         <f>0.0006 * sqrt(500 * F36) * vlookup('入力_出力'!$J$16,$S$3:$Z$6, 8, FALSE) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,3, FALSE) * VLOOKUP(switch('入力_出力'!$D$41,"Turf",'入力_出力'!$E$10,"Dirt",'入力_出力'!$H$10),'定義'!$B$3:$C$10,2, FALSE)</f>
-        <v>0.3219937888</v>
+        <v>0.3425833932</v>
       </c>
       <c r="E54" s="148">
         <f> (C54 - B54) / D54</f>
-        <v>10.55898482</v>
+        <v>11.42930246</v>
       </c>
       <c r="F54" s="140">
         <f> (B54 + C54) / 2 * E54</f>
-        <v>232.3610952</v>
+        <v>252.6317992</v>
       </c>
       <c r="G54" s="140">
         <f> 20 * B36 * B37 * ((B54 + D54 * E54 - B33 + 12) ^ 3 - (B54 - B33 + 12) ^ 3) / (3 * D54) / 144</f>
-        <v>365.7437451</v>
+        <v>413.3570199</v>
       </c>
     </row>
     <row r="55">
@@ -6820,23 +6820,23 @@
       </c>
       <c r="B55" s="153">
         <f> (B33 * (vlookup('入力_出力'!$J$16,$S$3:$Z$6, 5, FALSE) + 0.01) + sqrt(500 * F34) * VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,2, FALSE) * 0.002) * 1.05 + sqrt(500 * F34) *VLOOKUP(switch('入力_出力'!$J$42,"Sprint",'入力_出力'!$E$12,"Mile",'入力_出力'!$H$12,"Medium",'入力_出力'!$K$12,"Long",'入力_出力'!$N$12),'定義'!$E$3:$G$10,2, FALSE) * 0.002</f>
-        <v>23.70597089</v>
+        <v>24.06161316</v>
       </c>
       <c r="C55" s="25"/>
       <c r="D55" s="157" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E55" s="148">
         <f> F55 / B55</f>
-        <v>12.69605196</v>
+        <v>11.66594826</v>
       </c>
       <c r="F55" s="140">
         <f> '入力_出力'!D42/ 3 - F54</f>
-        <v>300.9722381</v>
+        <v>280.7015341</v>
       </c>
       <c r="G55" s="140">
         <f> 20 * B36 *B37* (B55 - B33 + 12) ^ 2 / 144 * E55</f>
-        <v>553.6429997</v>
+        <v>547.3532822</v>
       </c>
     </row>
     <row r="56">
@@ -6846,7 +6846,7 @@
       <c r="F56" s="25"/>
       <c r="G56" s="160">
         <f>SUM(G41:G45)+SUM(G54:G55)</f>
-        <v>1963.146833</v>
+        <v>2005.996916</v>
       </c>
     </row>
     <row r="57">
@@ -6856,7 +6856,7 @@
       <c r="F57" s="25"/>
       <c r="G57" s="141">
         <f>F35+(G56-B35)/0.8/vlookup('入力_出力'!$J$16,$S$3:$Z$6, 2, FALSE)/ (1 + ($K$33+$K$34) / 10000)</f>
-        <v>453.9335406</v>
+        <v>570.2203876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>